<commit_message>
Perubahan awal dari versi saya
</commit_message>
<xml_diff>
--- a/public/Data Layanan.xlsx
+++ b/public/Data Layanan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yudapramana/Sites/ptsp.kemenagpessel/public/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\sipintuv1\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BBF8E45-EFF4-DB40-88F2-3741435CD091}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63EB1DED-EF3A-4B5F-BCE8-9E170C36BBE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{B64A1DCE-EE3A-194B-B1D2-B270E2BBB9D0}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{B64A1DCE-EE3A-194B-B1D2-B270E2BBB9D0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,17 +19,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -932,21 +921,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE692555-352E-BC45-845A-68614F977634}">
   <dimension ref="A2:G114"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="A113" sqref="A113:XFD114"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.19921875" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="65" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="40.5" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="33" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="43.33203125" style="3" customWidth="1"/>
-    <col min="6" max="7" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="43.296875" style="3" customWidth="1"/>
+    <col min="6" max="7" width="13.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -969,7 +958,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -992,7 +981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -1015,7 +1004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>3</v>
       </c>
@@ -1038,7 +1027,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>4</v>
       </c>
@@ -1061,7 +1050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>5</v>
       </c>
@@ -1084,7 +1073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>6</v>
       </c>
@@ -1107,7 +1096,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>7</v>
       </c>
@@ -1130,7 +1119,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>8</v>
       </c>
@@ -1153,7 +1142,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>9</v>
       </c>
@@ -1176,7 +1165,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>10</v>
       </c>
@@ -1199,7 +1188,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>11</v>
       </c>
@@ -1222,7 +1211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>12</v>
       </c>
@@ -1245,7 +1234,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>13</v>
       </c>
@@ -1268,7 +1257,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>14</v>
       </c>
@@ -1291,7 +1280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>15</v>
       </c>
@@ -1314,7 +1303,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>16</v>
       </c>
@@ -1337,7 +1326,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>17</v>
       </c>
@@ -1360,7 +1349,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>18</v>
       </c>
@@ -1383,7 +1372,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>19</v>
       </c>
@@ -1406,7 +1395,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>20</v>
       </c>
@@ -1429,7 +1418,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>21</v>
       </c>
@@ -1452,7 +1441,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <v>22</v>
       </c>
@@ -1475,7 +1464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>23</v>
       </c>
@@ -1498,7 +1487,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
         <v>24</v>
       </c>
@@ -1521,7 +1510,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
         <v>25</v>
       </c>
@@ -1544,7 +1533,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
         <v>26</v>
       </c>
@@ -1567,7 +1556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
         <v>27</v>
       </c>
@@ -1590,7 +1579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
         <v>28</v>
       </c>
@@ -1613,7 +1602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
         <v>29</v>
       </c>
@@ -1636,7 +1625,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="3">
         <v>30</v>
       </c>
@@ -1659,7 +1648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="3">
         <v>31</v>
       </c>
@@ -1682,7 +1671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="3">
         <v>32</v>
       </c>
@@ -1705,7 +1694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="3">
         <v>33</v>
       </c>
@@ -1728,7 +1717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="3">
         <v>34</v>
       </c>
@@ -1751,7 +1740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="3">
         <v>35</v>
       </c>
@@ -1774,7 +1763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="3">
         <v>36</v>
       </c>
@@ -1797,7 +1786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="3">
         <v>37</v>
       </c>
@@ -1820,7 +1809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="3">
         <v>38</v>
       </c>
@@ -1843,7 +1832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="3">
         <v>39</v>
       </c>
@@ -1866,7 +1855,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="3">
         <v>40</v>
       </c>
@@ -1889,7 +1878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="3">
         <v>41</v>
       </c>
@@ -1912,7 +1901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="3">
         <v>42</v>
       </c>
@@ -1935,7 +1924,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="3">
         <v>43</v>
       </c>
@@ -1958,7 +1947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="3">
         <v>44</v>
       </c>
@@ -1981,7 +1970,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="3">
         <v>45</v>
       </c>
@@ -2004,7 +1993,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="3">
         <v>46</v>
       </c>
@@ -2027,7 +2016,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="3">
         <v>47</v>
       </c>
@@ -2050,7 +2039,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="3">
         <v>48</v>
       </c>
@@ -2073,7 +2062,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" s="3">
         <v>49</v>
       </c>
@@ -2096,7 +2085,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" s="3">
         <v>50</v>
       </c>
@@ -2119,7 +2108,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" s="3">
         <v>51</v>
       </c>
@@ -2142,7 +2131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" s="3">
         <v>52</v>
       </c>
@@ -2165,7 +2154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" s="3">
         <v>53</v>
       </c>
@@ -2188,7 +2177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" s="3">
         <v>54</v>
       </c>
@@ -2211,7 +2200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" s="3">
         <v>55</v>
       </c>
@@ -2234,7 +2223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" s="3">
         <v>56</v>
       </c>
@@ -2257,7 +2246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" s="3">
         <v>57</v>
       </c>
@@ -2280,7 +2269,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" s="3">
         <v>58</v>
       </c>
@@ -2303,7 +2292,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" s="3">
         <v>59</v>
       </c>
@@ -2326,7 +2315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" s="3">
         <v>60</v>
       </c>
@@ -2349,7 +2338,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" s="3">
         <v>61</v>
       </c>
@@ -2372,7 +2361,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" s="3">
         <v>62</v>
       </c>
@@ -2395,7 +2384,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" s="3">
         <v>63</v>
       </c>
@@ -2418,7 +2407,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" s="3">
         <v>64</v>
       </c>
@@ -2441,7 +2430,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" s="3">
         <v>65</v>
       </c>
@@ -2464,7 +2453,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" s="3">
         <v>66</v>
       </c>
@@ -2487,7 +2476,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" s="3">
         <v>67</v>
       </c>
@@ -2510,7 +2499,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" s="3">
         <v>68</v>
       </c>
@@ -2533,7 +2522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71" s="3">
         <v>69</v>
       </c>
@@ -2556,7 +2545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" s="3">
         <v>70</v>
       </c>
@@ -2579,7 +2568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A73" s="3">
         <v>71</v>
       </c>
@@ -2602,7 +2591,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A74" s="3">
         <v>72</v>
       </c>
@@ -2625,7 +2614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A75" s="3">
         <v>73</v>
       </c>
@@ -2648,7 +2637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A76" s="3">
         <v>74</v>
       </c>
@@ -2671,7 +2660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A77" s="3">
         <v>75</v>
       </c>
@@ -2694,7 +2683,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A78" s="3">
         <v>76</v>
       </c>
@@ -2717,7 +2706,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A79" s="3">
         <v>77</v>
       </c>
@@ -2740,7 +2729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A80" s="3">
         <v>78</v>
       </c>
@@ -2763,7 +2752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A81" s="3">
         <v>79</v>
       </c>
@@ -2786,7 +2775,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A82" s="3">
         <v>80</v>
       </c>
@@ -2809,7 +2798,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A83" s="3">
         <v>81</v>
       </c>
@@ -2832,7 +2821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A84" s="3">
         <v>82</v>
       </c>
@@ -2855,7 +2844,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A85" s="3">
         <v>83</v>
       </c>
@@ -2878,7 +2867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A86" s="3">
         <v>84</v>
       </c>
@@ -2901,7 +2890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A87" s="3">
         <v>85</v>
       </c>
@@ -2924,7 +2913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A88" s="3">
         <v>86</v>
       </c>
@@ -2947,7 +2936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A89" s="3">
         <v>87</v>
       </c>
@@ -2970,7 +2959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A90" s="3">
         <v>88</v>
       </c>
@@ -2993,7 +2982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A91" s="3">
         <v>89</v>
       </c>
@@ -3016,7 +3005,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A92" s="3">
         <v>90</v>
       </c>
@@ -3039,7 +3028,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A93" s="3">
         <v>91</v>
       </c>
@@ -3062,7 +3051,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A94" s="3">
         <v>92</v>
       </c>
@@ -3085,7 +3074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A95" s="3">
         <v>93</v>
       </c>
@@ -3108,7 +3097,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A96" s="3">
         <v>94</v>
       </c>
@@ -3131,7 +3120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A97" s="3">
         <v>95</v>
       </c>
@@ -3154,7 +3143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A98" s="3">
         <v>96</v>
       </c>
@@ -3177,7 +3166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A99" s="3">
         <v>97</v>
       </c>
@@ -3200,7 +3189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A100" s="3">
         <v>98</v>
       </c>
@@ -3223,7 +3212,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A101" s="3">
         <v>99</v>
       </c>
@@ -3246,7 +3235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A102" s="3">
         <v>100</v>
       </c>
@@ -3269,7 +3258,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A103" s="3">
         <v>101</v>
       </c>
@@ -3292,7 +3281,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A104" s="3">
         <v>102</v>
       </c>
@@ -3315,7 +3304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A105" s="3">
         <v>103</v>
       </c>
@@ -3338,7 +3327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A106" s="3">
         <v>104</v>
       </c>
@@ -3361,7 +3350,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A107" s="3">
         <v>105</v>
       </c>
@@ -3384,7 +3373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A108" s="3">
         <v>106</v>
       </c>
@@ -3407,7 +3396,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A109" s="3">
         <v>107</v>
       </c>
@@ -3430,7 +3419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A110" s="3">
         <v>108</v>
       </c>
@@ -3453,7 +3442,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A111" s="3">
         <v>109</v>
       </c>
@@ -3476,7 +3465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A112" s="3">
         <v>110</v>
       </c>
@@ -3499,7 +3488,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A113" s="3">
         <v>111</v>
       </c>
@@ -3522,7 +3511,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A114" s="3">
         <v>112</v>
       </c>

</xml_diff>